<commit_message>
Adding changes in smoke
</commit_message>
<xml_diff>
--- a/download/bulk_user_details.xlsx
+++ b/download/bulk_user_details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Client Id</t>
   </si>
@@ -41,40 +41,55 @@
     <t>Role</t>
   </si>
   <si>
-    <t>WbfuR431</t>
-  </si>
-  <si>
-    <t>nhauqon87</t>
-  </si>
-  <si>
-    <t>e38#VvE$</t>
+    <t>UJLnj648</t>
+  </si>
+  <si>
+    <t>usomuin80</t>
+  </si>
+  <si>
+    <t>u#A74V!n</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>ldhwuJFq</t>
-  </si>
-  <si>
-    <t>fnJC</t>
+    <t>XCqBUXBb</t>
+  </si>
+  <si>
+    <t>NJae</t>
   </si>
   <si>
     <t>Candidate</t>
   </si>
   <si>
-    <t>Kjyvo596</t>
-  </si>
-  <si>
-    <t>njfvoeq85</t>
-  </si>
-  <si>
-    <t>C9nh$2%A</t>
-  </si>
-  <si>
-    <t>aHYKTxAE</t>
-  </si>
-  <si>
-    <t>mruj</t>
+    <t>opEDi265</t>
+  </si>
+  <si>
+    <t>pptaghb76</t>
+  </si>
+  <si>
+    <t>eTC7u&amp;2$</t>
+  </si>
+  <si>
+    <t>ENpBoHRd</t>
+  </si>
+  <si>
+    <t>dFMq</t>
+  </si>
+  <si>
+    <t>GaiRe814</t>
+  </si>
+  <si>
+    <t>fafepfu81</t>
+  </si>
+  <si>
+    <t>c7C9N!#p</t>
+  </si>
+  <si>
+    <t>OBLxNjot</t>
+  </si>
+  <si>
+    <t>gZgz</t>
   </si>
 </sst>
 </file>
@@ -442,10 +457,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:H3"/>
+      <selection activeCell="A1" sqref="A1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -481,7 +496,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>231106302</v>
+        <v>23110820</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
@@ -507,7 +522,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="2">
-        <v>231106301</v>
+        <v>23110819</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -525,6 +540,32 @@
         <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2">
+        <v>23110818</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
newly added font end TCs
</commit_message>
<xml_diff>
--- a/download/bulk_user_details.xlsx
+++ b/download/bulk_user_details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Client Id</t>
   </si>
@@ -41,25 +41,55 @@
     <t>Role</t>
   </si>
   <si>
-    <t>aGKBW286</t>
-  </si>
-  <si>
-    <t>nhfldgk95</t>
-  </si>
-  <si>
-    <t>wr3V9!$M</t>
+    <t>omLKn912</t>
+  </si>
+  <si>
+    <t>ngayxqc48</t>
+  </si>
+  <si>
+    <t>Rf&amp;N5n!8</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>ASiXJWbN</t>
-  </si>
-  <si>
-    <t>WKRh</t>
+    <t>UjDHiFTq</t>
+  </si>
+  <si>
+    <t>ezdS</t>
   </si>
   <si>
     <t>Candidate</t>
+  </si>
+  <si>
+    <t>sEdlG343</t>
+  </si>
+  <si>
+    <t>uymwjkw37</t>
+  </si>
+  <si>
+    <t>hm65%E#P</t>
+  </si>
+  <si>
+    <t>xZVPOvsr</t>
+  </si>
+  <si>
+    <t>WvJv</t>
+  </si>
+  <si>
+    <t>iUkOr451</t>
+  </si>
+  <si>
+    <t>sghlmrc51</t>
+  </si>
+  <si>
+    <t>xF&amp;N3$2k</t>
+  </si>
+  <si>
+    <t>ffHADbov</t>
+  </si>
+  <si>
+    <t>fpzh</t>
   </si>
 </sst>
 </file>
@@ -427,10 +457,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:H2"/>
+      <selection activeCell="A1" sqref="A1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -466,7 +496,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>23111603</v>
+        <v>2012454353</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
@@ -484,6 +514,58 @@
         <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2012454354</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2012454355</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>